<commit_message>
Added interesting experiments to mlp
</commit_message>
<xml_diff>
--- a/src/models/mlp_model_results.xlsx
+++ b/src/models/mlp_model_results.xlsx
@@ -8,21 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCL_CS\Y3\COMP0029 Individual Project\Individual Project (90%)\UCL-FYP\src\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8665024-CC16-4C33-A0F0-14BEA2632A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831E2104-D349-4D3E-98BF-8B17D16B3B3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8F14163F-E633-4BD5-ABD0-DA53CD420175}"/>
+    <workbookView xWindow="-14145" yWindow="2580" windowWidth="14385" windowHeight="12255" firstSheet="1" activeTab="2" xr2:uid="{8F14163F-E633-4BD5-ABD0-DA53CD420175}"/>
   </bookViews>
   <sheets>
     <sheet name="MLP 6b,c" sheetId="1" r:id="rId1"/>
+    <sheet name="MLP 7a" sheetId="2" r:id="rId2"/>
+    <sheet name="MLP 7b" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'MLP 6b,c'!#REF!</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'MLP 6b,c'!#REF!</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'MLP 6b,c'!#REF!</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'MLP 6b,c'!$C$1:$C$28</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'MLP 6b,c'!$D$1:$D$28</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'MLP 6b,c'!$E$1:$E$28</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -44,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="40">
   <si>
     <t>Trial 1</t>
   </si>
@@ -93,6 +87,78 @@
   <si>
     <t>avg best k (continuous)</t>
   </si>
+  <si>
+    <t>Block 1</t>
+  </si>
+  <si>
+    <t>Block 2</t>
+  </si>
+  <si>
+    <t>Block 3</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Bottle1</t>
+  </si>
+  <si>
+    <t>Bottle2</t>
+  </si>
+  <si>
+    <t>Bottle3</t>
+  </si>
+  <si>
+    <t>Cylinder1</t>
+  </si>
+  <si>
+    <t>Cylinder2</t>
+  </si>
+  <si>
+    <t>Cylinder3</t>
+  </si>
+  <si>
+    <t>k=11</t>
+  </si>
+  <si>
+    <t>k=1</t>
+  </si>
+  <si>
+    <t>k=5</t>
+  </si>
+  <si>
+    <t>k=16</t>
+  </si>
+  <si>
+    <t>k=20</t>
+  </si>
+  <si>
+    <t>Randomly sample dataset and train on MLP</t>
+  </si>
+  <si>
+    <t>Sample size</t>
+  </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>overall</t>
+  </si>
+  <si>
+    <t>*k=11 for PCA</t>
+  </si>
+  <si>
+    <t>*T=Train, V=Validate</t>
+  </si>
+  <si>
+    <t>Accuracy (5 trials) with varying k components for PCA</t>
+  </si>
+  <si>
+    <t>Accuracies</t>
+  </si>
 </sst>
 </file>
 
@@ -115,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -132,15 +198,138 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,7 +704,1021 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>MLP accuracy v.s.</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> randomised dataset sample size</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MLP 7b'!$C$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MLP 7b'!$C$6:$C$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>71.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>73.75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>79.290000000000006</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84.38</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>83.33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>84.55</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>89.62</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>88.93</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8F9-44A0-924D-BCFC6C50D61D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MLP 7b'!$D$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MLP 7b'!$D$6:$D$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>78.33</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D8F9-44A0-924D-BCFC6C50D61D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MLP 7b'!$E$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MLP 7b'!$E$6:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>72.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86.67</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>80.83</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78.569999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D8F9-44A0-924D-BCFC6C50D61D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MLP 7b'!$F$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 4</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MLP 7b'!$F$6:$F$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>82.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.67</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>82.14</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-D8F9-44A0-924D-BCFC6C50D61D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MLP 7b'!$G$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Trial 5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MLP 7b'!$G$6:$G$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>71.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.33</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.709999999999994</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80.62</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81.67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>89.5</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>86.82</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>84.17</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>88.46</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>85</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D8F9-44A0-924D-BCFC6C50D61D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'MLP 7b'!$H$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>AVG</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent6"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'MLP 7b'!$H$6:$H$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="14"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.334000000000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>75.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>78.831999999999994</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.569999999999993</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33.700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34.274000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>33.667999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>35.616</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>34.786000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-D8F9-44A0-924D-BCFC6C50D61D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1750089839"/>
+        <c:axId val="1750097519"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1750089839"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Dataset</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> sample size (hundreds)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750097519"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1750097519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Accuracy</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750089839"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1058,6 +2261,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1079,6 +2785,47 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3FCF749-D1A4-48E2-E8B5-8457D3498BD7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F424603C-66DE-E005-07BF-E5316AD0CC87}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1398,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF1CB94C-E1CE-4D59-ADA5-49270B9C5680}">
   <dimension ref="B3:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -1409,25 +3156,25 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1557,33 +3304,33 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>1</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11">
         <v>67.709999999999994</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>66.319999999999993</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>60.76</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11">
         <v>73.260000000000005</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11">
         <v>63.89</v>
       </c>
       <c r="H11" s="1">
@@ -1595,19 +3342,19 @@
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12">
         <v>67.010000000000005</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>68.06</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>67.709999999999994</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12">
         <v>67.709999999999994</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12">
         <v>62.5</v>
       </c>
       <c r="H12" s="1">
@@ -1619,19 +3366,19 @@
       <c r="B13">
         <v>3</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13">
         <v>73.959999999999994</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>70</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>77.08</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13">
         <v>71.180000000000007</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13">
         <v>72.569999999999993</v>
       </c>
       <c r="H13" s="1">
@@ -1643,19 +3390,19 @@
       <c r="B14">
         <v>4</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14">
         <v>70.14</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>70.489999999999995</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>65.97</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14">
         <v>76.040000000000006</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14">
         <v>69.44</v>
       </c>
       <c r="H14" s="1">
@@ -1667,19 +3414,19 @@
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15">
         <v>73.61</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>72.569999999999993</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>67.36</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15">
         <v>69.099999999999994</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15">
         <v>70.489999999999995</v>
       </c>
       <c r="H15" s="1">
@@ -1691,19 +3438,19 @@
       <c r="B16">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16">
         <v>73.260000000000005</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>70.489999999999995</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>77.08</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16">
         <v>72.2</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16">
         <v>77.08</v>
       </c>
       <c r="H16" s="1">
@@ -1715,19 +3462,19 @@
       <c r="B17">
         <v>7</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17">
         <v>70.83</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>75.69</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>70.14</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17">
         <v>75</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17">
         <v>74.650000000000006</v>
       </c>
       <c r="H17" s="1">
@@ -1739,19 +3486,19 @@
       <c r="B18">
         <v>8</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18">
         <v>71.180000000000007</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>73.260000000000005</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>72.569999999999993</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18">
         <v>71.88</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18">
         <v>73.61</v>
       </c>
       <c r="H18" s="1">
@@ -1763,19 +3510,19 @@
       <c r="B19">
         <v>9</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19">
         <v>69.44</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>69.790000000000006</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>73.959999999999994</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19">
         <v>72.92</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19">
         <v>69.44</v>
       </c>
       <c r="H19" s="1">
@@ -1787,19 +3534,19 @@
       <c r="B20">
         <v>10</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20">
         <v>69.790000000000006</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>72.92</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>73.959999999999994</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20">
         <v>75.349999999999994</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20">
         <v>77.430000000000007</v>
       </c>
       <c r="H20" s="1">
@@ -1811,19 +3558,19 @@
       <c r="B21">
         <v>11</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21">
         <v>76.040000000000006</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>75</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>71.53</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21">
         <v>72.569999999999993</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21">
         <v>75.349999999999994</v>
       </c>
       <c r="H21" s="1">
@@ -1835,19 +3582,19 @@
       <c r="B22">
         <v>12</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22">
         <v>73.959999999999994</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>72.569999999999993</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>74.650000000000006</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22">
         <v>69.099999999999994</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22">
         <v>74.31</v>
       </c>
       <c r="H22" s="1">
@@ -1859,19 +3606,19 @@
       <c r="B23">
         <v>13</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23">
         <v>72.569999999999993</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>72.92</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>70.489999999999995</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23">
         <v>72.569999999999993</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23">
         <v>64.239999999999995</v>
       </c>
       <c r="H23" s="1">
@@ -1883,19 +3630,19 @@
       <c r="B24">
         <v>14</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24">
         <v>67.36</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
         <v>75.349999999999994</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>72.22</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24">
         <v>72.569999999999993</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24">
         <v>74.650000000000006</v>
       </c>
       <c r="H24" s="1">
@@ -1907,19 +3654,19 @@
       <c r="B25">
         <v>15</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25">
         <v>71.53</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25">
         <v>73.959999999999994</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
         <v>71.88</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25">
         <v>73.260000000000005</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25">
         <v>70.83</v>
       </c>
       <c r="H25" s="1">
@@ -1931,19 +3678,19 @@
       <c r="B26">
         <v>16</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26">
         <v>77.430000000000007</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26">
         <v>72.92</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>69.44</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26">
         <v>69.44</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26">
         <v>66.319999999999993</v>
       </c>
       <c r="H26" s="1">
@@ -1955,19 +3702,19 @@
       <c r="B27">
         <v>17</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27">
         <v>71.180000000000007</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27">
         <v>67.36</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>72.92</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27">
         <v>68.75</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27">
         <v>70.489999999999995</v>
       </c>
       <c r="H27" s="1">
@@ -1979,19 +3726,19 @@
       <c r="B28">
         <v>18</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28">
         <v>69.790000000000006</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28">
         <v>76.040000000000006</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28">
         <v>72.22</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28">
         <v>69.099999999999994</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28">
         <v>68.06</v>
       </c>
       <c r="H28" s="1">
@@ -2003,19 +3750,19 @@
       <c r="B29">
         <v>19</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29">
         <v>70.489999999999995</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29">
         <v>72.22</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>68.75</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29">
         <v>74.650000000000006</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29">
         <v>71.88</v>
       </c>
       <c r="H29" s="1">
@@ -2027,19 +3774,19 @@
       <c r="B30">
         <v>20</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30">
         <v>73.260000000000005</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
         <v>72.22</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>75.349999999999994</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30">
         <v>69.790000000000006</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30">
         <v>68.75</v>
       </c>
       <c r="H30" s="1">
@@ -2134,4 +3881,913 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C585EC34-F14A-4548-8F33-C537A7FD0E32}">
+  <dimension ref="C1:L22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="12">
+        <v>56.87</v>
+      </c>
+      <c r="G5" s="13">
+        <v>52</v>
+      </c>
+      <c r="H5" s="13">
+        <v>51.38</v>
+      </c>
+      <c r="I5" s="13">
+        <v>51.62</v>
+      </c>
+      <c r="J5" s="14">
+        <v>48.63</v>
+      </c>
+      <c r="K5" s="1">
+        <f>AVERAGE(F5:J5)</f>
+        <v>52.1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="12">
+        <v>52.25</v>
+      </c>
+      <c r="G6" s="13">
+        <v>53.87</v>
+      </c>
+      <c r="H6" s="13">
+        <v>57.5</v>
+      </c>
+      <c r="I6" s="13">
+        <v>57.13</v>
+      </c>
+      <c r="J6" s="14">
+        <v>55.25</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" ref="K6:K7" si="0">AVERAGE(F6:J6)</f>
+        <v>55.2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="15">
+        <v>52.5</v>
+      </c>
+      <c r="G7" s="5">
+        <v>62.63</v>
+      </c>
+      <c r="H7" s="5">
+        <v>56.25</v>
+      </c>
+      <c r="I7" s="5">
+        <v>56.88</v>
+      </c>
+      <c r="J7" s="16">
+        <v>55.12</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="0"/>
+        <v>56.676000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="17">
+        <f>AVERAGE(F5:F7)</f>
+        <v>53.873333333333335</v>
+      </c>
+      <c r="G8" s="4">
+        <f t="shared" ref="G8:J8" si="1">AVERAGE(G5:G7)</f>
+        <v>56.166666666666664</v>
+      </c>
+      <c r="H8" s="4">
+        <f t="shared" si="1"/>
+        <v>55.043333333333329</v>
+      </c>
+      <c r="I8" s="4">
+        <f t="shared" si="1"/>
+        <v>55.21</v>
+      </c>
+      <c r="J8" s="18">
+        <f t="shared" si="1"/>
+        <v>53</v>
+      </c>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H10" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="12">
+        <v>51</v>
+      </c>
+      <c r="G11" s="13">
+        <v>54.25</v>
+      </c>
+      <c r="H11" s="13">
+        <v>57.37</v>
+      </c>
+      <c r="I11" s="13">
+        <v>65.13</v>
+      </c>
+      <c r="J11" s="14">
+        <v>55.62</v>
+      </c>
+      <c r="K11" s="1">
+        <f>AVERAGE(F11:J11)</f>
+        <v>56.673999999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="12">
+        <v>54.75</v>
+      </c>
+      <c r="G12" s="13">
+        <v>54.62</v>
+      </c>
+      <c r="H12" s="13">
+        <v>49.375</v>
+      </c>
+      <c r="I12" s="13">
+        <v>57.87</v>
+      </c>
+      <c r="J12" s="14">
+        <v>44.13</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" ref="K12:K13" si="2">AVERAGE(F12:J12)</f>
+        <v>52.149000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="15">
+        <v>51.25</v>
+      </c>
+      <c r="G13" s="5">
+        <v>57.5</v>
+      </c>
+      <c r="H13" s="5">
+        <v>61.75</v>
+      </c>
+      <c r="I13" s="5">
+        <v>60.87</v>
+      </c>
+      <c r="J13" s="16">
+        <v>59.13</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="2"/>
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="17">
+        <f>AVERAGE(F11:F13)</f>
+        <v>52.333333333333336</v>
+      </c>
+      <c r="G14" s="4">
+        <f t="shared" ref="G14:J14" si="3">AVERAGE(G11:G13)</f>
+        <v>55.456666666666671</v>
+      </c>
+      <c r="H14" s="4">
+        <f t="shared" si="3"/>
+        <v>56.164999999999999</v>
+      </c>
+      <c r="I14" s="4">
+        <f t="shared" si="3"/>
+        <v>61.29</v>
+      </c>
+      <c r="J14" s="18">
+        <f t="shared" si="3"/>
+        <v>52.96</v>
+      </c>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F15" s="12"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="12">
+        <v>49.63</v>
+      </c>
+      <c r="G17" s="13">
+        <v>42.5</v>
+      </c>
+      <c r="H17" s="13">
+        <v>49.38</v>
+      </c>
+      <c r="I17" s="13">
+        <v>52.87</v>
+      </c>
+      <c r="J17" s="14">
+        <v>50.25</v>
+      </c>
+      <c r="K17" s="1">
+        <f>AVERAGE(F17:J17)</f>
+        <v>48.926000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="12">
+        <v>49.25</v>
+      </c>
+      <c r="G18" s="13">
+        <v>53.38</v>
+      </c>
+      <c r="H18" s="13">
+        <v>53.63</v>
+      </c>
+      <c r="I18" s="13">
+        <v>48.75</v>
+      </c>
+      <c r="J18" s="14">
+        <v>45.87</v>
+      </c>
+      <c r="K18" s="1">
+        <f t="shared" ref="K18:K19" si="4">AVERAGE(F18:J18)</f>
+        <v>50.176000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="15">
+        <v>51.75</v>
+      </c>
+      <c r="G19" s="5">
+        <v>51</v>
+      </c>
+      <c r="H19" s="5">
+        <v>46</v>
+      </c>
+      <c r="I19" s="5">
+        <v>58.25</v>
+      </c>
+      <c r="J19" s="16">
+        <v>44.13</v>
+      </c>
+      <c r="K19" s="1">
+        <f t="shared" si="4"/>
+        <v>50.225999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="17">
+        <f>AVERAGE(F17:F19)</f>
+        <v>50.21</v>
+      </c>
+      <c r="G20" s="4">
+        <f t="shared" ref="G20:J20" si="5">AVERAGE(G17:G19)</f>
+        <v>48.96</v>
+      </c>
+      <c r="H20" s="4">
+        <f t="shared" si="5"/>
+        <v>49.669999999999995</v>
+      </c>
+      <c r="I20" s="4">
+        <f t="shared" si="5"/>
+        <v>53.29</v>
+      </c>
+      <c r="J20" s="18">
+        <f t="shared" si="5"/>
+        <v>46.75</v>
+      </c>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="F21" s="12"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+    </row>
+    <row r="22" spans="3:12" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="15">
+        <f>AVERAGE(F8,F14,F20)</f>
+        <v>52.138888888888893</v>
+      </c>
+      <c r="G22" s="5">
+        <f>AVERAGE(G8,G14,G20)</f>
+        <v>53.527777777777779</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" ref="H22:J22" si="6">AVERAGE(H8,H14,H20)</f>
+        <v>53.626111111111108</v>
+      </c>
+      <c r="I22" s="5">
+        <f t="shared" si="6"/>
+        <v>56.596666666666664</v>
+      </c>
+      <c r="J22" s="16">
+        <f t="shared" si="6"/>
+        <v>50.903333333333336</v>
+      </c>
+      <c r="L22" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53D69161-649E-4639-AF87-A27D4975AF83}">
+  <dimension ref="B2:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>100</v>
+      </c>
+      <c r="C6" s="1">
+        <v>45</v>
+      </c>
+      <c r="D6" s="1">
+        <v>50</v>
+      </c>
+      <c r="E6" s="1">
+        <v>60</v>
+      </c>
+      <c r="F6" s="1">
+        <v>75</v>
+      </c>
+      <c r="G6" s="1">
+        <v>70</v>
+      </c>
+      <c r="H6" s="1">
+        <f>AVERAGE(C6:G6)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>200</v>
+      </c>
+      <c r="C7" s="1">
+        <v>60</v>
+      </c>
+      <c r="D7" s="1">
+        <v>67.5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>72.5</v>
+      </c>
+      <c r="F7" s="1">
+        <v>67.5</v>
+      </c>
+      <c r="G7" s="1">
+        <v>65</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7:H19" si="0">AVERAGE(C7:G7)</f>
+        <v>66.5</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>300</v>
+      </c>
+      <c r="C8" s="1">
+        <v>71.67</v>
+      </c>
+      <c r="D8" s="1">
+        <v>78.33</v>
+      </c>
+      <c r="E8" s="1">
+        <v>86.67</v>
+      </c>
+      <c r="F8" s="1">
+        <v>75</v>
+      </c>
+      <c r="G8" s="1">
+        <v>65</v>
+      </c>
+      <c r="H8" s="1">
+        <f t="shared" si="0"/>
+        <v>75.334000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>400</v>
+      </c>
+      <c r="C9" s="1">
+        <v>73.75</v>
+      </c>
+      <c r="D9" s="1">
+        <v>71.25</v>
+      </c>
+      <c r="E9" s="1">
+        <v>76.25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>82.5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>71.25</v>
+      </c>
+      <c r="H9" s="1">
+        <f t="shared" si="0"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>500</v>
+      </c>
+      <c r="C10" s="1">
+        <v>73</v>
+      </c>
+      <c r="D10" s="1">
+        <v>79</v>
+      </c>
+      <c r="E10" s="1">
+        <v>79</v>
+      </c>
+      <c r="F10" s="1">
+        <v>73</v>
+      </c>
+      <c r="G10" s="1">
+        <v>75</v>
+      </c>
+      <c r="H10" s="1">
+        <f t="shared" si="0"/>
+        <v>75.8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>600</v>
+      </c>
+      <c r="C11" s="1">
+        <v>80.83</v>
+      </c>
+      <c r="D11" s="1">
+        <v>77.5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>80.83</v>
+      </c>
+      <c r="F11" s="1">
+        <v>76.67</v>
+      </c>
+      <c r="G11" s="1">
+        <v>78.33</v>
+      </c>
+      <c r="H11" s="1">
+        <f t="shared" si="0"/>
+        <v>78.831999999999994</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>700</v>
+      </c>
+      <c r="C12" s="1">
+        <v>79.290000000000006</v>
+      </c>
+      <c r="D12" s="1">
+        <v>82.14</v>
+      </c>
+      <c r="E12" s="1">
+        <v>78.569999999999993</v>
+      </c>
+      <c r="F12" s="1">
+        <v>82.14</v>
+      </c>
+      <c r="G12" s="1">
+        <v>80.709999999999994</v>
+      </c>
+      <c r="H12" s="1">
+        <f t="shared" si="0"/>
+        <v>80.569999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>800</v>
+      </c>
+      <c r="C13" s="1">
+        <v>84.38</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>80.62</v>
+      </c>
+      <c r="H13" s="1">
+        <f>AVERAGE(C13:G13)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>900</v>
+      </c>
+      <c r="C14" s="1">
+        <v>83.33</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>81.67</v>
+      </c>
+      <c r="H14" s="1">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>1000</v>
+      </c>
+      <c r="C15" s="1">
+        <v>79</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>89.5</v>
+      </c>
+      <c r="H15" s="1">
+        <f t="shared" si="0"/>
+        <v>33.700000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <v>1100</v>
+      </c>
+      <c r="C16" s="1">
+        <v>84.55</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>86.82</v>
+      </c>
+      <c r="H16" s="1">
+        <f t="shared" si="0"/>
+        <v>34.274000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17">
+        <v>1200</v>
+      </c>
+      <c r="C17" s="1">
+        <v>84.17</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>84.17</v>
+      </c>
+      <c r="H17" s="1">
+        <f t="shared" si="0"/>
+        <v>33.667999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>1300</v>
+      </c>
+      <c r="C18" s="1">
+        <v>89.62</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>88.46</v>
+      </c>
+      <c r="H18" s="1">
+        <f t="shared" si="0"/>
+        <v>35.616</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>1400</v>
+      </c>
+      <c r="C19" s="1">
+        <v>88.93</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>85</v>
+      </c>
+      <c r="H19" s="1">
+        <f t="shared" si="0"/>
+        <v>34.786000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>